<commit_message>
Added files related to ridge regression
</commit_message>
<xml_diff>
--- a/UK-Sales_Predictive_Model/2017/6. LM with Weather + Lasso/Output_Data/Lasso_Weather_Output_analyzed_2017.xlsx
+++ b/UK-Sales_Predictive_Model/2017/6. LM with Weather + Lasso/Output_Data/Lasso_Weather_Output_analyzed_2017.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="384" windowWidth="22692" windowHeight="8940" activeTab="1"/>
+    <workbookView xWindow="288" yWindow="384" windowWidth="22692" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="Lasso_Weather_Output" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
-    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lasso_Weather_Output!$A$4:$J$121</definedName>
@@ -21,7 +20,7 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="53" r:id="rId5"/>
+    <pivotCache cacheId="58" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -1066,13 +1065,13 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1766,11 +1765,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="185126912"/>
-        <c:axId val="185128448"/>
+        <c:axId val="190532224"/>
+        <c:axId val="190562688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="185126912"/>
+        <c:axId val="190532224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1789,7 +1788,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185128448"/>
+        <c:crossAx val="190562688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1797,7 +1796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185128448"/>
+        <c:axId val="190562688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1807,7 +1806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185126912"/>
+        <c:crossAx val="190532224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3609,147 +3608,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Lasso_Weather_Output"/>
-      <sheetName val="UK FY16-FY17 WATERFALL"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="53">
-          <cell r="C53" t="str">
-            <v>Base Sales</v>
-          </cell>
-          <cell r="E53">
-            <v>103.14430177588201</v>
-          </cell>
-          <cell r="F53">
-            <v>416.60211018882489</v>
-          </cell>
-          <cell r="G53">
-            <v>27.476676368069263</v>
-          </cell>
-          <cell r="H53">
-            <v>4.2839569856184996</v>
-          </cell>
-          <cell r="K53" t="str">
-            <v>Base ($103, 7.5%)</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="C54" t="str">
-            <v>Holiday/Seasonality</v>
-          </cell>
-          <cell r="E54">
-            <v>551.5070453183946</v>
-          </cell>
-          <cell r="F54">
-            <v>705.30248196928824</v>
-          </cell>
-          <cell r="G54">
-            <v>103.2658116894884</v>
-          </cell>
-          <cell r="K54" t="str">
-            <v>Day of the Week ($417, 30.3%)</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="C55" t="str">
-            <v>Clearance</v>
-          </cell>
-          <cell r="E55">
-            <v>1360.0753389771712</v>
-          </cell>
-          <cell r="F55">
-            <v>58.34015727655833</v>
-          </cell>
-          <cell r="K55" t="str">
-            <v>Labor ($27, 2.%)</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="C56" t="str">
-            <v>B3G3</v>
-          </cell>
-          <cell r="E56">
-            <v>1418.4154962537295</v>
-          </cell>
-          <cell r="F56">
-            <v>51.686724529761726</v>
-          </cell>
-          <cell r="K56" t="str">
-            <v>Operating Hours ($4, .3%)</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="C57" t="str">
-            <v>Weather</v>
-          </cell>
-          <cell r="E57">
-            <v>1463.4956634196262</v>
-          </cell>
-          <cell r="F57">
-            <v>6.6065573638650665</v>
-          </cell>
-          <cell r="K57" t="str">
-            <v>Seasonality ($705, 51.2%)</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="C58" t="str">
-            <v>Other Promos</v>
-          </cell>
-          <cell r="E58">
-            <v>1377.1364999999998</v>
-          </cell>
-          <cell r="F58">
-            <v>86.35916341962637</v>
-          </cell>
-          <cell r="K58" t="str">
-            <v>Holiday ($103, 7.5%)</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="C59" t="str">
-            <v>Avg. Store Daily Sales</v>
-          </cell>
-          <cell r="E59">
-            <v>1377.1364999999998</v>
-          </cell>
-          <cell r="K59" t="str">
-            <v>Clearance ($58, 4.2%)</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="K60" t="str">
-            <v>B3G3 ($52, 3.8%)</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="K61" t="str">
-            <v>Weather (-$7, -.5%)</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="K62" t="str">
-            <v>Other Promos (-$86, -4.2%)</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="K63" t="str">
-            <v>$1,377
- Total Avg. Daily Store Sales</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Srini Aripirala" refreshedDate="43160.681765740737" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="117">
   <cacheSource type="worksheet">
@@ -5224,7 +5082,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="53" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="58" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="N6:O18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -5322,7 +5180,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable12" cacheId="53" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Waterfall Category">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable12" cacheId="58" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Waterfall Category">
   <location ref="C31:E49" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -5437,7 +5295,7 @@
     <dataField name="% to Total" fld="9" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="0">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
     <format dxfId="1">
@@ -5449,7 +5307,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -5755,10 +5613,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:O121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10005,12 +9864,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="C6:K63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A14" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>

</xml_diff>